<commit_message>
Updated all the functionalities
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-AuditLogs.data.xlsx
+++ b/tests/artifact/data/UI-AuditLogs.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="184">
   <si>
     <t>login.screen</t>
   </si>
@@ -496,13 +496,13 @@
     <t>From.DateValues</t>
   </si>
   <si>
-    <t>17-10-2023</t>
+    <t>26-11-2023</t>
   </si>
   <si>
     <t>To.DateValues</t>
   </si>
   <si>
-    <t>19-10-2023</t>
+    <t>27-11-2023</t>
   </si>
   <si>
     <t>NonFin.From.Date</t>
@@ -563,6 +563,38 @@
   </si>
   <si>
     <t>//main[@class='mb-5']/section/div[2]/table/tbody/tr/td[1]</t>
+  </si>
+  <si>
+    <t>Filter.PopUp</t>
+  </si>
+  <si>
+    <t>//*[@class='popover-body']</t>
+  </si>
+  <si>
+    <t>Search.Values</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF212529"/>
+        <rFont val="Segoe UI"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Category Updated: TestCategory431</t>
+    </r>
+  </si>
+  <si>
+    <t>searchResult.values</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/table/tbody/tr[1]/td[1]</t>
+  </si>
+  <si>
+    <t>Invalid.result</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]</t>
   </si>
 </sst>
 </file>
@@ -575,7 +607,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -616,6 +648,12 @@
       <sz val="10.5"/>
       <color rgb="FF5F6368"/>
       <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1090,152 +1128,152 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1264,6 +1302,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1677,10 +1718,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C88"/>
+  <dimension ref="A1:C92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -2398,6 +2439,38 @@
         <v>175</v>
       </c>
     </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="90" ht="17.5" spans="1:2">
+      <c r="A90" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A25">

</xml_diff>

<commit_message>
Updated Audit Logs script
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-AuditLogs.data.xlsx
+++ b/tests/artifact/data/UI-AuditLogs.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="186">
   <si>
     <t>login.screen</t>
   </si>
@@ -595,6 +595,12 @@
   </si>
   <si>
     <t>//main[@class='mb-5']/section/div[2]</t>
+  </si>
+  <si>
+    <t>Valid.numbers</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div[2]/td[1]</t>
   </si>
 </sst>
 </file>
@@ -1718,7 +1724,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:C93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A77" workbookViewId="0">
       <selection activeCell="A93" sqref="A93"/>
@@ -2471,6 +2477,14 @@
         <v>183</v>
       </c>
     </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A25">

</xml_diff>